<commit_message>
Created a Master Data file for NYS
</commit_message>
<xml_diff>
--- a/Data/2010_average_income.xlsx
+++ b/Data/2010_average_income.xlsx
@@ -283,12 +283,12 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,7 +626,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>